<commit_message>
2017-10-10: change recordInfo format to field:value; rewrite test case from nodeunit to mocha
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24180" windowHeight="14070" activeTab="4"/>
+    <workbookView windowWidth="24135" windowHeight="12630" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162">
   <si>
     <t>rc</t>
   </si>
@@ -1460,6 +1460,12 @@
   </si>
   <si>
     <t>51000~51100</t>
+  </si>
+  <si>
+    <t>penalize</t>
+  </si>
+  <si>
+    <t>51100~51200</t>
   </si>
   <si>
     <t>redis</t>
@@ -1479,9 +1485,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -1509,37 +1515,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1559,14 +1542,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -1581,9 +1556,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1594,37 +1568,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1642,6 +1585,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1651,7 +1650,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1666,7 +1672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1678,25 +1684,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1709,54 +1697,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1816,13 +1756,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1850,6 +1808,54 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -1857,6 +1863,54 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1878,23 +1932,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1924,186 +1963,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3235,10 +3241,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:D29"/>
+  <dimension ref="A2:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -3377,8 +3383,19 @@
       <c r="A29" t="s">
         <v>154</v>
       </c>
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
       <c r="C29" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3401,16 +3418,16 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017-11-08: recreate create impeach logic with compund field check
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24135" windowHeight="12630" activeTab="4"/>
+    <workbookView windowWidth="28695" windowHeight="12630" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165">
   <si>
     <t>rc</t>
   </si>
@@ -1453,6 +1453,9 @@
     </r>
   </si>
   <si>
+    <t>impeach_action(user)</t>
+  </si>
+  <si>
     <t>50900~51000</t>
   </si>
   <si>
@@ -1466,6 +1469,12 @@
   </si>
   <si>
     <t>51100~51200</t>
+  </si>
+  <si>
+    <t>impeach_action(adminUser)</t>
+  </si>
+  <si>
+    <t>51200~51300</t>
   </si>
   <si>
     <t>redis</t>
@@ -1515,20 +1524,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1536,6 +1544,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1550,14 +1588,62 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1565,28 +1651,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1601,63 +1665,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1672,19 +1681,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1696,25 +1729,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1732,13 +1753,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1750,19 +1783,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1774,13 +1807,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1798,19 +1831,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1822,7 +1843,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1834,25 +1855,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1863,15 +1872,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1886,30 +1886,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1932,8 +1908,37 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1953,13 +1958,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1968,148 +1977,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3241,15 +3250,16 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:D30"/>
+  <dimension ref="A2:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="3" width="11.45" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
+    <col min="3" max="3" width="11.45" customWidth="1"/>
     <col min="4" max="4" width="22.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3373,29 +3383,37 @@
     </row>
     <row r="27" spans="2:3">
       <c r="B27" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="B30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3418,16 +3436,16 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017-12-17: 1. add/modify validateFormat/value for part edit_sub_field, and realted test case; 2. modify valueMatchRuleDefineCheck in validateHelper, set all rule check result true for pass, false to fail; 3. add new function in controllerHelper:pushOptionalPartIntoExpectedPart_noReturn && getPartValue
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="194">
   <si>
     <t>rc</t>
   </si>
@@ -1580,6 +1580,268 @@
   </si>
   <si>
     <t>maintain(express_admin)-&gt;daily</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource_profile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10760~10800</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>51300~51400</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2029,7 +2291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -2432,10 +2694,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D42"/>
+  <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2682,52 +2944,60 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>108</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>109</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>110</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>112</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2838,10 +3108,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D31"/>
+  <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3007,10 +3277,62 @@
         <v>157</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2018-04-24: 1. add logout;2 ready to add folder
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12160" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -68,6 +69,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>和</t>
@@ -84,6 +86,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>一致，只是开头改成</t>
@@ -104,6 +107,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
@@ -118,6 +122,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
@@ -132,6 +137,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
@@ -146,6 +152,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -159,6 +166,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -172,6 +180,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -185,6 +194,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -198,6 +208,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -211,6 +222,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -224,6 +236,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -265,6 +278,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>上一个</t>
@@ -281,6 +295,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>正好以</t>
@@ -297,6 +312,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>的整数结尾，所以</t>
@@ -313,6 +329,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>后起始</t>
@@ -336,6 +353,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -344,6 +362,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -358,6 +377,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:字段级别的错误</t>
@@ -371,6 +391,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -379,6 +400,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -393,6 +415,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -401,6 +424,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -415,6 +439,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -423,6 +448,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -435,7 +461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="207">
   <si>
     <t>rc</t>
   </si>
@@ -445,6 +471,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>s</t>
@@ -454,6 +481,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ub rc</t>
@@ -465,6 +493,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>s</t>
@@ -474,6 +503,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ub-rc function</t>
@@ -494,6 +524,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>10000-1</t>
@@ -503,6 +534,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>9</t>
@@ -512,6 +544,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -523,6 +556,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>m</t>
@@ -532,6 +566,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ongoRule</t>
@@ -543,6 +578,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -552,6 +588,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0000-29999</t>
@@ -602,6 +639,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -611,6 +649,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -620,6 +659,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-3</t>
@@ -629,6 +669,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -638,6 +679,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -652,6 +694,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -661,6 +704,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>1</t>
@@ -670,6 +714,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-3</t>
@@ -679,6 +724,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>1</t>
@@ -688,6 +734,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -702,6 +749,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -711,6 +759,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -720,6 +769,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-3</t>
@@ -729,6 +779,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -738,6 +789,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -752,6 +804,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -761,6 +814,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0000～49999</t>
@@ -775,6 +829,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>40000-400</t>
@@ -784,6 +839,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>99</t>
@@ -804,6 +860,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>40</t>
@@ -813,6 +870,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -822,6 +880,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00-40</t>
@@ -831,6 +890,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -840,6 +900,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>99</t>
@@ -851,6 +912,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -860,6 +922,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ssist-&gt;crypt</t>
@@ -955,6 +1018,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -964,6 +1028,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>dmin</t>
@@ -975,6 +1040,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -984,6 +1050,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>dmin_user</t>
@@ -998,6 +1065,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -1007,6 +1075,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>dmin_sugar</t>
@@ -1018,6 +1087,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>1</t>
@@ -1027,6 +1097,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0030~10040</t>
@@ -1038,6 +1109,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>c</t>
@@ -1047,6 +1119,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ategory</t>
@@ -1070,6 +1143,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>100</t>
@@ -1079,6 +1153,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>8</t>
@@ -1088,6 +1163,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0~10100</t>
@@ -1108,6 +1184,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -1117,6 +1194,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>rticle</t>
@@ -1269,6 +1347,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>1</t>
@@ -1278,6 +1357,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0800~10830</t>
@@ -1418,6 +1498,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>50</t>
@@ -1427,6 +1508,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -1436,6 +1518,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~50700</t>
@@ -1447,6 +1530,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>507</t>
@@ -1456,6 +1540,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~50</t>
@@ -1465,6 +1550,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>8</t>
@@ -1474,6 +1560,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1483,6 +1570,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1497,6 +1585,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>508</t>
@@ -1506,6 +1595,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~50</t>
@@ -1515,6 +1605,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>9</t>
@@ -1524,6 +1615,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1533,6 +1625,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1571,6 +1664,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1580,6 +1674,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -1589,6 +1684,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1598,6 +1694,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -1607,6 +1704,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1616,6 +1714,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1627,6 +1726,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1636,6 +1736,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -1645,6 +1746,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1654,6 +1756,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -1663,6 +1766,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1672,6 +1776,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1683,6 +1788,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1692,6 +1798,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -1701,6 +1808,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1710,6 +1818,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>7</t>
@@ -1719,6 +1828,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1728,6 +1838,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1739,6 +1850,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1748,6 +1860,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>7</t>
@@ -1757,6 +1870,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1766,6 +1880,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>8</t>
@@ -1775,6 +1890,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00</t>
@@ -1784,9 +1900,6 @@
     <t>51800~51900</t>
   </si>
   <si>
-    <t>51900~52000</t>
-  </si>
-  <si>
     <t>redis</t>
   </si>
   <si>
@@ -1807,6 +1920,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>server_common</t>
@@ -1816,6 +1930,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>)-&gt;</t>
@@ -1825,6 +1940,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>checkRule</t>
@@ -1848,6 +1964,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -1857,6 +1974,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-4</t>
@@ -1866,6 +1984,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -1875,6 +1994,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>049</t>
@@ -1911,6 +2031,30 @@
   </si>
   <si>
     <t>preCheck</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>older</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51900~52000</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>52000~52100</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1929,12 +2073,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1942,6 +2088,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1949,11 +2096,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1971,6 +2120,7 @@
       <b/>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -2612,7 +2762,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,16 +2771,16 @@
         <v>50</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,10 +3339,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" t="s">
         <v>201</v>
-      </c>
-      <c r="C14" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3203,10 +3353,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D39"/>
+  <dimension ref="A2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3266,10 +3416,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,129 +3465,143 @@
         <v>169</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>108</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D25" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="D26" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>174</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>176</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>119</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>180</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>93</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>187</v>
+        <v>102</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>106</v>
       </c>
-      <c r="C39" t="s">
-        <v>188</v>
-      </c>
+      <c r="C40" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3459,16 +3623,16 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>189</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>190</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>191</v>
-      </c>
-      <c r="H2" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3489,18 +3653,18 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
         <v>197</v>
-      </c>
-      <c r="B2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
         <v>199</v>
-      </c>
-      <c r="B3" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2018-05-01: 1. re-orginze input check, try to unify; 2. error code not hard code, but base code+offset
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12160" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="db" sheetId="6" r:id="rId6"/>
     <sheet name="controllerHelper_Checker" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -432,7 +432,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ada</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -461,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="176">
   <si>
     <t>rc</t>
   </si>
@@ -971,9 +981,109 @@
     <t>maintain(express)-&gt;daily</t>
   </si>
   <si>
+    <t>42000-42049</t>
+  </si>
+  <si>
     <t>maintain(express_admin)-&gt;daily</t>
   </si>
   <si>
+    <t>42050-42099</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>maintain(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>server_common</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>checkRule</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>000-4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>049</t>
+    </r>
+  </si>
+  <si>
     <t>REST API</t>
   </si>
   <si>
@@ -1013,6 +1123,15 @@
     <t>uploadDefine</t>
   </si>
   <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>应用新格式</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1057,9 +1176,6 @@
     </r>
   </si>
   <si>
-    <t>10000~10030</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1090,28 +1206,6 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0030~10040</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
       <t>c</t>
     </r>
     <r>
@@ -1126,27 +1220,302 @@
     </r>
   </si>
   <si>
-    <t>10050~10060</t>
-  </si>
-  <si>
     <t>store_path</t>
   </si>
   <si>
-    <t>10060~10080</t>
-  </si>
-  <si>
     <t>admin_penalize</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>100</t>
+    <t>resource_profile</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>rticle</t>
+    </r>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>article_comment</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>like_dislike</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>article_attachment</t>
+  </si>
+  <si>
+    <t>article_image</t>
+  </si>
+  <si>
+    <t>friend</t>
+  </si>
+  <si>
+    <t>member_penalize</t>
+  </si>
+  <si>
+    <t>public_group</t>
+  </si>
+  <si>
+    <t>public_group_event</t>
+  </si>
+  <si>
+    <t>public_group_interaction</t>
+  </si>
+  <si>
+    <t>user_friend_group</t>
+  </si>
+  <si>
+    <t>user_public_group</t>
+  </si>
+  <si>
+    <t>add_friend</t>
+  </si>
+  <si>
+    <t>impeach</t>
+  </si>
+  <si>
+    <t>impeach_comment</t>
+  </si>
+  <si>
+    <t>impeach_state</t>
+  </si>
+  <si>
+    <t>记录impeach状态或者处理人的变化，以便形成历史记录（只有create/search，无update和delete）</t>
+  </si>
+  <si>
+    <t>impeach_image</t>
+  </si>
+  <si>
+    <t>impeach_attachment</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>user_operation</t>
+  </si>
+  <si>
+    <t>recommend</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>collection</t>
+  </si>
+  <si>
+    <t>statci</t>
+  </si>
+  <si>
+    <t>like_dislike_static</t>
+  </si>
+  <si>
+    <t>resource_profile_static</t>
+  </si>
+  <si>
+    <t>validate</t>
+  </si>
+  <si>
+    <t>40000-40100</t>
+  </si>
+  <si>
+    <t>40100-40300</t>
+  </si>
+  <si>
+    <t>40300-40400</t>
+  </si>
+  <si>
+    <t>crypt</t>
+  </si>
+  <si>
+    <t>40400-40500</t>
+  </si>
+  <si>
+    <t>gmImage</t>
+  </si>
+  <si>
+    <t>40500-40600</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>40600~40700</t>
+  </si>
+  <si>
+    <t>shaLua</t>
+  </si>
+  <si>
+    <t>40700~40800</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>40800~40900</t>
+  </si>
+  <si>
+    <t>40900~41000</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>41000~42000</t>
+  </si>
+  <si>
+    <t>mongodb</t>
+  </si>
+  <si>
+    <t>mongoError</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>30000~30099</t>
+  </si>
+  <si>
+    <t>err.errors</t>
+  </si>
+  <si>
+    <t>inputRule=&gt;validator</t>
+  </si>
+  <si>
+    <t>30100～30199</t>
+  </si>
+  <si>
+    <t>controller</t>
+  </si>
+  <si>
+    <t>50200~50300</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>50300~50400</t>
+  </si>
+  <si>
+    <t>uploadFile</t>
+  </si>
+  <si>
+    <t>50400~50500</t>
+  </si>
+  <si>
+    <t>likeDislike</t>
+  </si>
+  <si>
+    <t>50500~50600</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>older</t>
+    </r>
+  </si>
+  <si>
+    <t>52000~52100</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50700</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>507</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50</t>
     </r>
     <r>
       <rPr>
@@ -1166,903 +1535,395 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>0~10100</t>
-    </r>
-  </si>
-  <si>
-    <t>resource_profile</t>
-  </si>
-  <si>
-    <t>11100~11200</t>
-  </si>
-  <si>
-    <t>code使用完毕，直接从user_operation=&gt;collection往后推</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>rticle</t>
-    </r>
-  </si>
-  <si>
-    <t>article</t>
-  </si>
-  <si>
-    <t>10100~10170</t>
-  </si>
-  <si>
-    <t>article_comment</t>
-  </si>
-  <si>
-    <t>10170~10190</t>
-  </si>
-  <si>
-    <t>folder</t>
-  </si>
-  <si>
-    <t>10190~10210</t>
-  </si>
-  <si>
-    <t>like_dislike</t>
-  </si>
-  <si>
-    <t>10210~10220</t>
-  </si>
-  <si>
-    <t>tags</t>
-  </si>
-  <si>
-    <t>10220~10230</t>
-  </si>
-  <si>
-    <t>article_attachment</t>
-  </si>
-  <si>
-    <t>10230~10260</t>
-  </si>
-  <si>
-    <t>article_image</t>
-  </si>
-  <si>
-    <t>10260~10290</t>
-  </si>
-  <si>
-    <t>friend</t>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>50700~50750 for user;50750~50800 for admin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>508</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>impeach_action(user)</t>
+  </si>
+  <si>
+    <t>50900~51000</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>51000~51100</t>
+  </si>
+  <si>
+    <t>penalize</t>
+  </si>
+  <si>
+    <t>51100~51200</t>
+  </si>
+  <si>
+    <t>impeach_action(adminUser)</t>
+  </si>
+  <si>
+    <t>51200~51300</t>
+  </si>
+  <si>
+    <t>51300~51400</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00</t>
+    </r>
+  </si>
+  <si>
+    <t>51800~51900</t>
+  </si>
+  <si>
+    <t>51900~52000</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>32000~33000</t>
+  </si>
+  <si>
+    <t>mongo</t>
+  </si>
+  <si>
+    <t>30000~31000</t>
+  </si>
+  <si>
+    <t>checker</t>
+  </si>
+  <si>
+    <t>preCheck</t>
+  </si>
+  <si>
+    <t>dispatch</t>
+  </si>
+  <si>
+    <t>resourceCheck</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>member_penalize</t>
-  </si>
-  <si>
-    <t>10300~10330</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>public_group</t>
-  </si>
-  <si>
-    <t>10330~10360</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>public_group_event</t>
-  </si>
-  <si>
-    <t>10360~10390</t>
-  </si>
-  <si>
-    <t>public_group_interaction</t>
-  </si>
-  <si>
-    <t>10390~10410</t>
-  </si>
-  <si>
-    <t>user_friend_group</t>
-  </si>
-  <si>
-    <t>10410~10430</t>
-  </si>
-  <si>
-    <t>user_public_group</t>
-  </si>
-  <si>
-    <t>10430~10440</t>
-  </si>
-  <si>
-    <t>add_friend</t>
-  </si>
-  <si>
-    <t>10440~10460</t>
-  </si>
-  <si>
-    <t>impeach</t>
-  </si>
-  <si>
-    <t>10500~10560</t>
-  </si>
-  <si>
-    <t>impeach_comment</t>
-  </si>
-  <si>
-    <t>10560~10590</t>
-  </si>
-  <si>
-    <t>impeach_state</t>
-  </si>
-  <si>
-    <t>10590~10610</t>
-  </si>
-  <si>
-    <t>记录impeach状态或者处理人的变化，以便形成历史记录（只有create/search，无update和delete）</t>
-  </si>
-  <si>
-    <t>impeach_image</t>
-  </si>
-  <si>
-    <t>10610~10640</t>
-  </si>
-  <si>
-    <t>impeach_attachment</t>
-  </si>
-  <si>
-    <t>10650~10700</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>10700~10740</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
-    <t>10740~10760</t>
-  </si>
-  <si>
-    <t>10760~10800</t>
-  </si>
-  <si>
-    <t>user_operation</t>
-  </si>
-  <si>
-    <t>recommend</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0800~10830</t>
-    </r>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>10830~10860</t>
-  </si>
-  <si>
-    <t>collection</t>
-  </si>
-  <si>
-    <t>10860~10890</t>
-  </si>
-  <si>
-    <t>statci</t>
-  </si>
-  <si>
-    <t>like_dislike_static</t>
-  </si>
-  <si>
-    <t>11200~11210</t>
-  </si>
-  <si>
-    <t>resource_profile占用了11100~11200</t>
-  </si>
-  <si>
-    <t>resource_profile_static</t>
-  </si>
-  <si>
-    <t>11210~11230</t>
-  </si>
-  <si>
-    <t>validate</t>
-  </si>
-  <si>
-    <t>40000-40100</t>
-  </si>
-  <si>
-    <t>40100-40300</t>
-  </si>
-  <si>
-    <t>40300-40400</t>
-  </si>
-  <si>
-    <t>crypt</t>
-  </si>
-  <si>
-    <t>40400-40500</t>
-  </si>
-  <si>
-    <t>gmImage</t>
-  </si>
-  <si>
-    <t>40500-40600</t>
-  </si>
-  <si>
-    <t>upload</t>
-  </si>
-  <si>
-    <t>40600~40700</t>
-  </si>
-  <si>
-    <t>shaLua</t>
-  </si>
-  <si>
-    <t>40700~40800</t>
-  </si>
-  <si>
-    <t>misc</t>
-  </si>
-  <si>
-    <t>40800~40900</t>
-  </si>
-  <si>
-    <t>40900~41000</t>
-  </si>
-  <si>
-    <t>mongodb</t>
-  </si>
-  <si>
-    <t>mongoError</t>
-  </si>
-  <si>
-    <t>common</t>
-  </si>
-  <si>
-    <t>30000~30099</t>
-  </si>
-  <si>
-    <t>err.errors</t>
-  </si>
-  <si>
-    <t>inputRule=&gt;validator</t>
-  </si>
-  <si>
-    <t>30100～30199</t>
-  </si>
-  <si>
-    <t>controller</t>
-  </si>
-  <si>
-    <t>60000~61000</t>
-  </si>
-  <si>
-    <t>checker</t>
-  </si>
-  <si>
-    <t>61000~62000</t>
-  </si>
-  <si>
-    <t>50200~50300</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>50300~50400</t>
-  </si>
-  <si>
-    <t>uploadFile</t>
-  </si>
-  <si>
-    <t>50400~50500</t>
-  </si>
-  <si>
-    <t>likeDislike</t>
-  </si>
-  <si>
-    <t>50500~50600</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~50700</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>507</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <t>50700~50750 for user;50750~50800 for admin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>508</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <t>impeach_action(user)</t>
-  </si>
-  <si>
-    <t>50900~51000</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>51000~51100</t>
-  </si>
-  <si>
-    <t>penalize</t>
-  </si>
-  <si>
-    <t>51100~51200</t>
-  </si>
-  <si>
-    <t>impeach_action(adminUser)</t>
-  </si>
-  <si>
-    <t>51200~51300</t>
-  </si>
-  <si>
-    <t>51300~51400</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~51</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00</t>
-    </r>
-  </si>
-  <si>
-    <t>51800~51900</t>
-  </si>
-  <si>
-    <t>redis</t>
-  </si>
-  <si>
-    <t>32000~33000</t>
-  </si>
-  <si>
-    <t>mongo</t>
-  </si>
-  <si>
-    <t>30000~31000</t>
-  </si>
-  <si>
-    <r>
-      <t>maintain(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>server_common</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>)-&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>checkRule</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>42050-42099</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>42000-42049</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>000-4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>049</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>helper</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>60000~61000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>checker</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>61000~62000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>security</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>41000~42000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>62000~63000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>preCheck</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>older</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>51900~52000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>52000~52100</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2072,6 +1933,13 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2146,23 +2014,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2534,10 +2403,10 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -2551,25 +2420,25 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4"/>
@@ -2582,23 +2451,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9" t="s">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="10">
         <v>20000</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
@@ -2610,19 +2479,19 @@
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="4"/>
@@ -2631,7 +2500,7 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="4"/>
@@ -2640,7 +2509,7 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="4"/>
@@ -2649,7 +2518,7 @@
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="4"/>
@@ -2661,7 +2530,7 @@
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="4"/>
@@ -2671,7 +2540,7 @@
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2680,7 +2549,7 @@
       <c r="C18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2689,134 +2558,134 @@
       <c r="C19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>194</v>
+      <c r="D27" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>193</v>
+      <c r="C28" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>195</v>
+      <c r="C29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="2"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2828,7 +2697,7 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="1"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
@@ -2837,14 +2706,14 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E39" s="4"/>
     </row>
@@ -2858,28 +2727,28 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
-      <c r="E42" s="6"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B43" s="4">
         <v>70000</v>
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="6">
+    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="7">
         <v>80000</v>
       </c>
-      <c r="C44" s="6"/>
+      <c r="C44" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId1"/>
@@ -2901,7 +2770,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>50000</v>
@@ -2909,24 +2778,24 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>50100</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2936,313 +2805,477 @@
     <col min="3" max="3" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="C2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>100099</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C3" s="5">
+        <v>100100</v>
+      </c>
+      <c r="D3">
+        <v>100199</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C4" s="2">
+        <v>100200</v>
+      </c>
+      <c r="D4">
+        <v>100299</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C5" s="2">
+        <v>100300</v>
+      </c>
+      <c r="D5">
+        <v>100399</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C6" s="5">
+        <v>100400</v>
+      </c>
+      <c r="D6">
+        <v>100499</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C7" s="2">
+        <v>100500</v>
+      </c>
+      <c r="D7">
+        <v>100599</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>101000</v>
+      </c>
+      <c r="D9">
+        <v>101099</v>
+      </c>
+      <c r="F9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>81</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>101100</v>
+      </c>
+      <c r="D10">
+        <v>101199</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11">
+        <v>101200</v>
+      </c>
+      <c r="D11">
+        <v>101299</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>83</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12">
+        <v>101300</v>
+      </c>
+      <c r="D12">
+        <v>101399</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="C13">
+        <v>101400</v>
+      </c>
+      <c r="D13">
+        <v>101499</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>85</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14">
+        <v>101500</v>
+      </c>
+      <c r="D14">
+        <v>101599</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C15">
+        <v>101600</v>
+      </c>
+      <c r="D15">
+        <v>101699</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>94</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20">
+        <v>102100</v>
+      </c>
+      <c r="D20">
+        <v>102199</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21">
+        <v>102200</v>
+      </c>
+      <c r="D21">
+        <v>102299</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22">
+        <v>102300</v>
+      </c>
+      <c r="D22">
+        <v>102399</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23">
+        <v>102400</v>
+      </c>
+      <c r="D23">
+        <v>102499</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24">
+        <v>102500</v>
+      </c>
+      <c r="D24">
+        <v>102599</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25">
+        <v>102600</v>
+      </c>
+      <c r="D25">
+        <v>102699</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26">
+        <v>102700</v>
+      </c>
+      <c r="D26">
+        <v>102799</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29">
+        <v>103100</v>
+      </c>
+      <c r="D29">
+        <v>103199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>96</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C30">
+        <v>103200</v>
+      </c>
+      <c r="D30">
+        <v>103299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C31">
+        <v>103300</v>
+      </c>
+      <c r="D31">
+        <v>103399</v>
+      </c>
+      <c r="E31" t="s">
         <v>98</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C32">
+        <v>103400</v>
+      </c>
+      <c r="D32">
+        <v>103499</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>100</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C33">
+        <v>103500</v>
+      </c>
+      <c r="D33">
+        <v>103599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" t="s">
-        <v>122</v>
+        <v>101</v>
+      </c>
+      <c r="C35">
+        <v>104100</v>
+      </c>
+      <c r="D35">
+        <v>104199</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>102</v>
+      </c>
+      <c r="C36">
+        <v>104200</v>
+      </c>
+      <c r="D36">
+        <v>104299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37">
+        <v>104300</v>
+      </c>
+      <c r="D37">
+        <v>104399</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>128</v>
+      <c r="A39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39">
+        <v>105100</v>
+      </c>
+      <c r="D39">
+        <v>105199</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>131</v>
-      </c>
-      <c r="B43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" t="s">
-        <v>134</v>
+      <c r="B40" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40">
+        <v>105200</v>
+      </c>
+      <c r="D40">
+        <v>105299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41">
+        <v>105300</v>
+      </c>
+      <c r="D41">
+        <v>105399</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>107</v>
+      </c>
       <c r="B44" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" t="s">
-        <v>136</v>
+        <v>108</v>
+      </c>
+      <c r="C44">
+        <v>106100</v>
+      </c>
+      <c r="D44">
+        <v>106199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45">
+        <v>106200</v>
+      </c>
+      <c r="D45">
+        <v>106299</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3263,70 +3296,70 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>138</v>
+      <c r="C2" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>139</v>
+      <c r="C3" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>140</v>
+      <c r="C4" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3334,19 +3367,19 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3355,8 +3388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3368,66 +3401,42 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" t="s">
-        <v>202</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3438,173 +3447,173 @@
         <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>206</v>
+      <c r="B23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>170</v>
+        <v>95</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>164</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>171</v>
+        <v>136</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>166</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>173</v>
+        <v>138</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>174</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>175</v>
+        <v>148</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>180</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>181</v>
+        <v>154</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>182</v>
+        <v>88</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>183</v>
+        <v>89</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>184</v>
+        <v>90</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>185</v>
+        <v>91</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>186</v>
+        <v>92</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>205</v>
+        <v>94</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
+      <c r="A42" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <legacyDrawing r:id="rId1"/>
@@ -3623,52 +3632,92 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" t="s">
-        <v>199</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>60000</v>
+      </c>
+      <c r="D4">
+        <v>60099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5">
+        <v>61000</v>
+      </c>
+      <c r="D5">
+        <v>60199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6">
+        <v>62000</v>
+      </c>
+      <c r="D6">
+        <v>60299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7">
+        <v>63000</v>
+      </c>
+      <c r="D7">
+        <v>60399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8">
+        <v>64000</v>
+      </c>
+      <c r="D8">
+        <v>60499</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2018-06-18:1. impeach code and test done
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="178">
   <si>
     <t>rc</t>
   </si>
@@ -1340,16 +1340,7 @@
     <t>impeach_comment</t>
   </si>
   <si>
-    <t>impeach_state</t>
-  </si>
-  <si>
-    <t>记录impeach状态或者处理人的变化，以便形成历史记录（只有create/search，无update和delete）</t>
-  </si>
-  <si>
     <t>impeach_image</t>
-  </si>
-  <si>
-    <t>impeach_attachment</t>
   </si>
   <si>
     <t>user</t>
@@ -1951,6 +1942,62 @@
   </si>
   <si>
     <t>public_group_event</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>impeach_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>action</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录impeach处理动作变化，以便形成历史记录（只有create/search，无update和delete）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>impeach_comment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>_image</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>impeach_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>attachment</t>
+    </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2847,10 +2894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2885,7 +2932,7 @@
         <v>100099</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2899,7 +2946,7 @@
         <v>100199</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2913,7 +2960,7 @@
         <v>100299</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2927,7 +2974,7 @@
         <v>100399</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2941,7 +2988,7 @@
         <v>100499</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,7 +3002,7 @@
         <v>100599</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2990,7 +3037,7 @@
         <v>101199</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,7 +3051,7 @@
         <v>101299</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3018,7 +3065,7 @@
         <v>101399</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3032,7 +3079,7 @@
         <v>101499</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,7 +3093,7 @@
         <v>101599</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3060,7 +3107,7 @@
         <v>101699</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3081,12 +3128,12 @@
         <v>102199</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C21">
         <v>102200</v>
@@ -3095,12 +3142,12 @@
         <v>102299</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C22">
         <v>102300</v>
@@ -3109,12 +3156,12 @@
         <v>102399</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C23">
         <v>102400</v>
@@ -3123,7 +3170,7 @@
         <v>102499</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3137,7 +3184,7 @@
         <v>102599</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3151,7 +3198,7 @@
         <v>102699</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3165,7 +3212,7 @@
         <v>102799</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3181,6 +3228,9 @@
       <c r="D29">
         <v>103199</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -3192,10 +3242,13 @@
       <c r="D30">
         <v>103299</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>97</v>
+      <c r="B31" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="C31">
         <v>103300</v>
@@ -3203,13 +3256,13 @@
       <c r="D31">
         <v>103399</v>
       </c>
-      <c r="E31" t="s">
-        <v>98</v>
+      <c r="F31" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>99</v>
+      <c r="B32" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="C32">
         <v>103400</v>
@@ -3217,10 +3270,16 @@
       <c r="D32">
         <v>103499</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C33">
         <v>103500</v>
@@ -3228,101 +3287,118 @@
       <c r="D33">
         <v>103599</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="F33" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34">
+        <v>103600</v>
+      </c>
+      <c r="D34">
+        <v>103699</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36">
+        <v>104100</v>
+      </c>
+      <c r="D36">
+        <v>104199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37">
+        <v>104200</v>
+      </c>
+      <c r="D37">
+        <v>104299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38">
+        <v>104300</v>
+      </c>
+      <c r="D38">
+        <v>104399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35">
-        <v>104100</v>
-      </c>
-      <c r="D35">
-        <v>104199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="C40">
+        <v>105100</v>
+      </c>
+      <c r="D40">
+        <v>105199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C36">
-        <v>104200</v>
-      </c>
-      <c r="D36">
-        <v>104299</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37">
-        <v>104300</v>
-      </c>
-      <c r="D37">
-        <v>104399</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="C41">
+        <v>105200</v>
+      </c>
+      <c r="D41">
+        <v>105299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C42">
+        <v>105300</v>
+      </c>
+      <c r="D42">
+        <v>105399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>104</v>
       </c>
-      <c r="C39">
-        <v>105100</v>
-      </c>
-      <c r="D39">
-        <v>105199</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="B45" t="s">
         <v>105</v>
       </c>
-      <c r="C40">
-        <v>105200</v>
-      </c>
-      <c r="D40">
-        <v>105299</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+      <c r="C45">
+        <v>106100</v>
+      </c>
+      <c r="D45">
+        <v>106199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>106</v>
       </c>
-      <c r="C41">
-        <v>105300</v>
-      </c>
-      <c r="D41">
-        <v>105399</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44">
-        <v>106100</v>
-      </c>
-      <c r="D44">
-        <v>106199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45">
+      <c r="C46">
         <v>106200</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>106299</v>
       </c>
     </row>
@@ -3351,13 +3427,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3365,7 +3441,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3373,48 +3449,48 @@
         <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3422,15 +3498,15 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3443,7 +3519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -3456,39 +3532,39 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
         <v>127</v>
-      </c>
-      <c r="B2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
         <v>60</v>
@@ -3502,40 +3578,40 @@
         <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3549,61 +3625,61 @@
         <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3614,7 +3690,7 @@
         <v>88</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3622,7 +3698,7 @@
         <v>89</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3630,7 +3706,7 @@
         <v>90</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3638,7 +3714,7 @@
         <v>91</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3646,7 +3722,7 @@
         <v>92</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,7 +3730,7 @@
         <v>93</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3662,7 +3738,7 @@
         <v>94</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3688,16 +3764,16 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" t="s">
         <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3729,7 +3805,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C5">
         <v>61000</v>
@@ -3740,7 +3816,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C6">
         <v>62000</v>
@@ -3751,7 +3827,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C7">
         <v>63000</v>
@@ -3762,7 +3838,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C8">
         <v>64000</v>

</xml_diff>

<commit_message>
2018-07-08: 1. user_friend_group code optimized && test case done: 2. optimze procedure of add_friend
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ss_vue_express\doc\错误代码\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="2"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -31,13 +26,12 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -45,14 +39,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1" shapeId="0">
+    <comment ref="A3" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -60,7 +54,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -69,7 +63,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>和</t>
@@ -78,7 +71,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -86,7 +79,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>一致，只是开头改成</t>
@@ -95,19 +87,18 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>2</t>
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
@@ -116,13 +107,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment ref="A13" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
@@ -131,13 +121,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0">
+    <comment ref="A14" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
@@ -146,13 +135,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0">
+    <comment ref="A16" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -160,13 +148,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="1" shapeId="0">
+    <comment ref="F36" authorId="1">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -174,13 +161,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="1" shapeId="0">
+    <comment ref="F37" authorId="1">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -188,13 +174,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="1" shapeId="0">
+    <comment ref="F39" authorId="1">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -202,13 +187,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="1" shapeId="0">
+    <comment ref="F40" authorId="1">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:
@@ -216,13 +200,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="0" shapeId="0">
+    <comment ref="A43" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -230,13 +213,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0" shapeId="0">
+    <comment ref="A44" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>zw:
@@ -254,14 +236,14 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -269,7 +251,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -278,7 +260,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>上一个</t>
@@ -287,7 +268,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -295,7 +276,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>正好以</t>
@@ -304,7 +284,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>10</t>
         </r>
@@ -312,7 +292,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>的整数结尾，所以</t>
@@ -321,7 +300,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -329,7 +308,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>后起始</t>
@@ -347,14 +325,13 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -363,7 +340,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -371,28 +347,26 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:字段级别的错误</t>
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -401,7 +375,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -409,14 +382,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -425,7 +397,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -433,24 +404,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="1" shapeId="0">
+    <comment ref="C21" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -458,9 +427,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>合并到article中</t>
@@ -477,14 +444,13 @@
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Ada:</t>
@@ -493,7 +459,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -506,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174">
   <si>
     <t>rc</t>
   </si>
@@ -516,7 +481,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>s</t>
@@ -526,7 +490,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ub rc</t>
@@ -538,7 +501,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>s</t>
@@ -548,7 +510,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ub-rc function</t>
@@ -569,7 +530,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>10000-1</t>
@@ -579,7 +539,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>9</t>
@@ -589,7 +548,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -601,7 +559,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>m</t>
@@ -611,7 +568,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ongoRule</t>
@@ -623,7 +579,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -633,7 +588,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0000-29999</t>
@@ -684,7 +638,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -694,7 +647,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -704,7 +656,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-3</t>
@@ -714,7 +665,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -724,7 +674,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -739,7 +688,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -749,7 +697,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>1</t>
@@ -759,7 +706,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-3</t>
@@ -769,7 +715,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>1</t>
@@ -779,7 +724,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -794,7 +738,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -804,7 +747,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -814,7 +756,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-3</t>
@@ -824,7 +765,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -834,7 +774,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>999</t>
@@ -849,7 +788,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -859,7 +797,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0000～49999</t>
@@ -874,7 +811,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>40000-400</t>
@@ -884,7 +820,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>99</t>
@@ -905,7 +840,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>40</t>
@@ -915,7 +849,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -925,7 +858,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00-40</t>
@@ -935,7 +867,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -945,7 +876,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>99</t>
@@ -957,7 +887,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -967,7 +896,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ssist-&gt;crypt</t>
@@ -1030,7 +958,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>maintain(</t>
@@ -1040,7 +967,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>server_common</t>
@@ -1050,7 +976,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>)-&gt;</t>
@@ -1060,7 +985,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>checkRule</t>
@@ -1072,7 +996,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -1082,7 +1005,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -1092,7 +1014,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>000-4</t>
@@ -1102,7 +1023,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -1112,7 +1032,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>049</t>
@@ -1172,7 +1091,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -1182,7 +1100,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>dmin</t>
@@ -1194,7 +1111,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -1204,19 +1120,20 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>dmin_user</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
+    <t>Y</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -1226,7 +1143,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>dmin_sugar</t>
@@ -1238,7 +1154,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>c</t>
@@ -1248,7 +1163,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ategory</t>
@@ -1269,7 +1183,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>a</t>
@@ -1279,7 +1192,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>rticle</t>
@@ -1289,9 +1201,6 @@
     <t>article</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>article_comment</t>
   </si>
   <si>
@@ -1313,6 +1222,9 @@
     <t>friend</t>
   </si>
   <si>
+    <t>add_friend</t>
+  </si>
+  <si>
     <t>member_penalize</t>
   </si>
   <si>
@@ -1331,7 +1243,10 @@
     <t>user_public_group</t>
   </si>
   <si>
-    <t>add_friend</t>
+    <t>join_public_group_request</t>
+  </si>
+  <si>
+    <t>to_be_friend_request</t>
   </si>
   <si>
     <t>impeach</t>
@@ -1340,9 +1255,72 @@
     <t>impeach_comment</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>impeach_comment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>_image</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>impeach_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>action</t>
+    </r>
+  </si>
+  <si>
+    <t>记录impeach处理动作变化，以便形成历史记录（只有create/search，无update和delete）</t>
+  </si>
+  <si>
     <t>impeach_image</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>impeach_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>attachment</t>
+    </r>
+  </si>
+  <si>
     <t>user</t>
   </si>
   <si>
@@ -1471,7 +1449,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>f</t>
@@ -1481,7 +1458,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>older</t>
@@ -1496,7 +1472,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>50</t>
@@ -1506,7 +1481,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -1516,7 +1490,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~50700</t>
@@ -1528,7 +1501,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>507</t>
@@ -1538,7 +1510,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~50</t>
@@ -1548,7 +1519,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>8</t>
@@ -1558,7 +1528,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1568,7 +1537,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1583,7 +1551,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>508</t>
@@ -1593,7 +1560,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~50</t>
@@ -1603,7 +1569,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>9</t>
@@ -1613,7 +1578,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1623,7 +1587,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1662,7 +1625,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1672,7 +1634,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -1682,7 +1643,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1692,7 +1652,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -1702,7 +1661,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1712,7 +1670,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1724,7 +1681,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1734,7 +1690,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -1744,7 +1699,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1754,7 +1708,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -1764,7 +1717,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1774,7 +1726,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1786,7 +1737,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1796,7 +1746,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -1806,7 +1755,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1816,7 +1764,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>7</t>
@@ -1826,7 +1773,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1836,7 +1782,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -1848,7 +1793,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>51</t>
@@ -1858,7 +1802,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>7</t>
@@ -1868,7 +1811,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00~51</t>
@@ -1878,7 +1820,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>8</t>
@@ -1888,7 +1829,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>00</t>
@@ -1923,89 +1863,19 @@
   </si>
   <si>
     <t>resourceCheck</t>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>member_penalize</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>public_group</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>public_group_event</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>impeach_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>action</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>记录impeach处理动作变化，以便形成历史记录（只有create/search，无update和delete）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>impeach_comment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>_image</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>impeach_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>attachment</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2013,24 +1883,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <strike/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2038,71 +1900,355 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2110,13 +2256,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2124,33 +2512,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2479,29 +2906,29 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.36328125" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="31.90625" customWidth="1"/>
-    <col min="4" max="4" width="29.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="42.6328125" customWidth="1"/>
+    <col min="1" max="1" width="30.3666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6333333333333" customWidth="1"/>
+    <col min="3" max="3" width="31.9083333333333" customWidth="1"/>
+    <col min="4" max="4" width="29.3666666666667" customWidth="1"/>
+    <col min="5" max="5" width="12.6333333333333" customWidth="1"/>
+    <col min="6" max="6" width="42.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2518,16 +2945,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2536,16 +2963,16 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4">
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2553,91 +2980,91 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
+    <row r="6" s="5" customFormat="1" spans="2:4">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" s="5" customFormat="1" spans="1:3">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>20000</v>
       </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="3:3">
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:3">
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" ht="14.15" customHeight="1" spans="2:4">
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -2646,7 +3073,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" ht="14.15" customHeight="1" spans="2:4">
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
         <v>31</v>
@@ -2655,116 +3082,116 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" ht="14.15" customHeight="1" spans="2:4">
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="4"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="4"/>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" s="4"/>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="4"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" s="4"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="B25" s="4"/>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="4"/>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" s="4"/>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="4"/>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" s="4"/>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" s="4"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="6"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4">
       <c r="B31" s="4"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2778,7 +3205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6">
       <c r="B33" s="4"/>
       <c r="C33" t="s">
         <v>59</v>
@@ -2790,48 +3217,51 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6">
       <c r="B36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6">
       <c r="B37" s="4"/>
       <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6">
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="2:6">
       <c r="B40" s="4"/>
       <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5">
       <c r="B42" s="4"/>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -2840,37 +3270,38 @@
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" s="2" customFormat="1" spans="1:3">
       <c r="A44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <v>80000</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.9083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2878,7 +3309,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2887,27 +3318,28 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:F34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="2" max="2" width="27.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.2666666666667" customWidth="1"/>
+    <col min="2" max="2" width="27.0916666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:6">
       <c r="C1" t="s">
         <v>68</v>
       </c>
@@ -2918,7 +3350,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -2931,27 +3363,27 @@
       <c r="D2">
         <v>100099</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
       <c r="B3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="5">
+        <v>74</v>
+      </c>
+      <c r="C3" s="3">
         <v>100100</v>
       </c>
       <c r="D3">
         <v>100199</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2">
         <v>100200</v>
@@ -2959,13 +3391,13 @@
       <c r="D4">
         <v>100299</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2">
         <v>100300</v>
@@ -2973,27 +3405,27 @@
       <c r="D5">
         <v>100399</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="5">
+        <v>77</v>
+      </c>
+      <c r="C6" s="3">
         <v>100400</v>
       </c>
       <c r="D6">
         <v>100499</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2">
         <v>100500</v>
@@ -3001,20 +3433,20 @@
       <c r="D7">
         <v>100599</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" ht="12.75" customHeight="1" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>101000</v>
@@ -3023,10 +3455,10 @@
         <v>101099</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" t="s">
         <v>81</v>
       </c>
@@ -3036,11 +3468,11 @@
       <c r="D10">
         <v>101199</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" t="s">
         <v>82</v>
       </c>
@@ -3050,11 +3482,11 @@
       <c r="D11">
         <v>101299</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" t="s">
         <v>83</v>
       </c>
@@ -3064,11 +3496,11 @@
       <c r="D12">
         <v>101399</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" t="s">
         <v>84</v>
       </c>
@@ -3078,11 +3510,11 @@
       <c r="D13">
         <v>101499</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" t="s">
         <v>85</v>
       </c>
@@ -3092,11 +3524,11 @@
       <c r="D14">
         <v>101599</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" t="s">
         <v>86</v>
       </c>
@@ -3106,20 +3538,20 @@
       <c r="D15">
         <v>101699</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" ht="12.75" customHeight="1"/>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C20">
         <v>102100</v>
@@ -3127,13 +3559,13 @@
       <c r="D20">
         <v>102199</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>169</v>
+      <c r="F20" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="C21">
         <v>102200</v>
@@ -3141,13 +3573,13 @@
       <c r="D21">
         <v>102299</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>171</v>
+      <c r="F21" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C22">
         <v>102300</v>
@@ -3155,13 +3587,13 @@
       <c r="D22">
         <v>102399</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>172</v>
+      <c r="F22" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="C23">
         <v>102400</v>
@@ -3169,13 +3601,13 @@
       <c r="D23">
         <v>102499</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C24">
         <v>102500</v>
@@ -3183,13 +3615,13 @@
       <c r="D24">
         <v>102599</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C25">
         <v>102600</v>
@@ -3197,13 +3629,13 @@
       <c r="D25">
         <v>102699</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C26">
         <v>102700</v>
@@ -3211,588 +3643,617 @@
       <c r="D26">
         <v>102799</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="F26" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" t="s">
         <v>95</v>
       </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29">
+      <c r="C27">
+        <v>102800</v>
+      </c>
+      <c r="D27">
+        <v>102899</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28">
+        <v>102900</v>
+      </c>
+      <c r="D28">
+        <v>102999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30">
         <v>103100</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>103199</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30">
+      <c r="F30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31">
         <v>103200</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>103299</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C31">
+      <c r="F31" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32">
         <v>103300</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>103399</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C32">
+      <c r="F32" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33">
         <v>103400</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>103499</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33">
+      <c r="E33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34">
         <v>103500</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>103599</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34">
+      <c r="F34" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35">
         <v>103600</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>103699</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36">
+      <c r="F35" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37">
         <v>104100</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>104199</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37">
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
         <v>104200</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>104299</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38">
+    <row r="39" spans="2:4">
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39">
         <v>104300</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>104399</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40">
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41">
         <v>105100</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <v>105199</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41">
+    <row r="42" spans="2:4">
+      <c r="B42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42">
         <v>105200</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>105299</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42">
+    <row r="43" spans="2:4">
+      <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43">
         <v>105300</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <v>105399</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45">
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46">
         <v>106100</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>106199</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46">
+    <row r="47" spans="2:4">
+      <c r="B47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47">
         <v>106200</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>106299</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="9.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.45" customWidth="1"/>
+    <col min="2" max="2" width="17.2666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.725" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:D42"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.2666666666667" customWidth="1"/>
+    <col min="3" max="3" width="11.45" customWidth="1"/>
+    <col min="4" max="4" width="23.2666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4">
       <c r="C3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4">
       <c r="D4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>135</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>87</v>
       </c>
       <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="C40" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
   <sheetData>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -3803,9 +4264,9 @@
         <v>60099</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C5">
         <v>61000</v>
@@ -3814,9 +4275,9 @@
         <v>60199</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C6">
         <v>62000</v>
@@ -3825,9 +4286,9 @@
         <v>60299</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C7">
         <v>63000</v>
@@ -3836,9 +4297,9 @@
         <v>60399</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C8">
         <v>64000</v>
@@ -3848,8 +4309,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2019-03-30: bug fix and code optimize
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="195">
   <si>
     <t>rc</t>
   </si>
@@ -1948,6 +1948,12 @@
   </si>
   <si>
     <t>52200~52299</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>33000~34000</t>
   </si>
 </sst>
 </file>
@@ -3540,7 +3546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -3792,31 +3798,45 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>154</v>
       </c>
       <c r="B2" t="s">
         <v>155</v>
       </c>
-      <c r="G2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H2" t="s">
-        <v>157</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2019-05-15: optimize some function
</commit_message>
<xml_diff>
--- a/doc/错误代码/错误代码范围.xlsx
+++ b/doc/错误代码/错误代码范围.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\ss_vue_express\doc\错误代码\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA691486-00FC-4EFF-AB9D-A02CA511CC67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -25,13 +26,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>zw</author>
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1" shapeId="0">
+    <comment ref="A3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -140,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="1" shapeId="0">
+    <comment ref="F36" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="1" shapeId="0">
+    <comment ref="F37" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -179,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="1" shapeId="0">
+    <comment ref="F39" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -192,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="1" shapeId="0">
+    <comment ref="F40" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="0" shapeId="0">
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -218,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0" shapeId="0">
+    <comment ref="A44" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -236,12 +237,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -324,13 +325,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ada</author>
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -352,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -365,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -387,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -409,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="1" shapeId="0">
+    <comment ref="C21" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -444,12 +445,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -476,7 +477,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="197">
   <si>
     <t>rc</t>
   </si>
@@ -1954,12 +1955,18 @@
   </si>
   <si>
     <t>33000~34000</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>41300~41400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2409,7 +2416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -2786,7 +2793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2821,7 +2828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -3376,11 +3383,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3454,85 +3461,93 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>169</v>
+      </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>186</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>175</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>176</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>177</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>178</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3543,7 +3558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -3797,10 +3812,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -3841,7 +3856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>